<commit_message>
Another bug bites the dust
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_component_Evaluation_series/first_release_qoq_DOMUSE.xlsx
+++ b/0_0_Data/2_Processed_Data/2_component_Evaluation_series/first_release_qoq_DOMUSE.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>value</t>
+    <t>first_release_value</t>
   </si>
   <si>
     <t>date</t>
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -399,418 +399,666 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>39400</v>
+        <v>38398</v>
       </c>
       <c r="B2">
-        <v>-0.8957516004554691</v>
+        <v>-1.019024872684525</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>39583</v>
+        <v>38487</v>
       </c>
       <c r="B3">
-        <v>1.910893826230975</v>
+        <v>0.8876024303436765</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>39765</v>
+        <v>38579</v>
       </c>
       <c r="B4">
-        <v>-0.9623800849065276</v>
+        <v>0.501281665261132</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>39948</v>
+        <v>38671</v>
       </c>
       <c r="B5">
-        <v>-1.734840982136873</v>
+        <v>0.783791364788172</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>40130</v>
+        <v>38763</v>
       </c>
       <c r="B6">
-        <v>-1.4178810011895</v>
+        <v>0.2322508451440228</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>40310</v>
+        <v>38852</v>
       </c>
       <c r="B7">
-        <v>-1.470147873721189</v>
+        <v>0.8665864397470244</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>40494</v>
+        <v>38944</v>
       </c>
       <c r="B8">
-        <v>1.938408417700344</v>
+        <v>0.6793221546917749</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>40676</v>
+        <v>39036</v>
       </c>
       <c r="B9">
-        <v>-0.163634158232469</v>
+        <v>-0.9228048723025069</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>40862</v>
+        <v>39128</v>
       </c>
       <c r="B10">
-        <v>0.4</v>
+        <v>1.742611766026243</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>41044</v>
+        <v>39217</v>
       </c>
       <c r="B11">
-        <v>-0.3</v>
+        <v>-0.8957516004554691</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>41228</v>
+        <v>39309</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.893923595129948</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>41409</v>
+        <v>39401</v>
       </c>
       <c r="B13">
-        <v>0.009235986179263023</v>
+        <v>-0.2567725410682868</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>41592</v>
+        <v>39493</v>
       </c>
       <c r="B14">
-        <v>0.3863474960573257</v>
+        <v>1.910893826230975</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>41774</v>
+        <v>39583</v>
       </c>
       <c r="B15">
-        <v>1.852186157158073</v>
+        <v>-0.9623800849065276</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>41957</v>
+        <v>39675</v>
       </c>
       <c r="B16">
-        <v>-0.1726927221574073</v>
+        <v>1.320073940737448</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>42137</v>
+        <v>39767</v>
       </c>
       <c r="B17">
-        <v>1.050807574684342</v>
+        <v>-0.05810994121875979</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>42321</v>
+        <v>39859</v>
       </c>
       <c r="B18">
-        <v>-0.2184803162966205</v>
+        <v>-1.734840982136873</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>42503</v>
+        <v>39948</v>
       </c>
       <c r="B19">
-        <v>0.8513884674671885</v>
+        <v>-1.4178810011895</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>42689</v>
+        <v>40040</v>
       </c>
       <c r="B20">
-        <v>0.4819278240608753</v>
+        <v>1.258487819346726</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>42867</v>
+        <v>40132</v>
       </c>
       <c r="B21">
-        <v>0.6629265129002277</v>
+        <v>-1.470147873721189</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>43053</v>
+        <v>40224</v>
       </c>
       <c r="B22">
-        <v>1.164700738417963</v>
+        <v>1.38192517089017</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>43145</v>
+        <v>40313</v>
       </c>
       <c r="B23">
-        <v>0.3865811319001295</v>
+        <v>1.938408417700344</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>43235</v>
+        <v>40405</v>
       </c>
       <c r="B24">
-        <v>0.3857269132374052</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>43326</v>
+        <v>40497</v>
       </c>
       <c r="B25">
-        <v>0.4445645077595088</v>
+        <v>-0.163634158232469</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>43418</v>
+        <v>40589</v>
       </c>
       <c r="B26">
-        <v>0.7</v>
+        <v>1.079830393426633</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>43510</v>
+        <v>40678</v>
       </c>
       <c r="B27">
-        <v>0.764905301728362</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>43600</v>
+        <v>40770</v>
       </c>
       <c r="B28">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>43691</v>
+        <v>40862</v>
       </c>
       <c r="B29">
-        <v>-0.1011524282971408</v>
+        <v>0.2303676816657827</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>43783</v>
+        <v>40954</v>
       </c>
       <c r="B30">
-        <v>0.3399426662647187</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>43875</v>
+        <v>41044</v>
       </c>
       <c r="B31">
-        <v>-0.4401201376428787</v>
+        <v>-0.4045626487644824</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>43966</v>
+        <v>41136</v>
       </c>
       <c r="B32">
-        <v>-1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>44068</v>
+        <v>41228</v>
       </c>
       <c r="B33">
-        <v>-7.231044133207007</v>
+        <v>-0.01847206600469065</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>44159</v>
+        <v>41320</v>
       </c>
       <c r="B34">
-        <v>4.665333711727925</v>
+        <v>0.009235986179263023</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>44251</v>
+        <v>41409</v>
       </c>
       <c r="B35">
-        <v>-0.2672256391354182</v>
+        <v>0.3863474960573257</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>44341</v>
+        <v>41501</v>
       </c>
       <c r="B36">
-        <v>-1.26956845314902</v>
+        <v>0.6964197943645729</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>44432</v>
+        <v>41593</v>
       </c>
       <c r="B37">
-        <v>2.350117300589673</v>
+        <v>-0.3183250015702015</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>44525</v>
+        <v>41685</v>
       </c>
       <c r="B38">
-        <v>2.031122027629067</v>
+        <v>1.852186157158073</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>44617</v>
+        <v>41774</v>
       </c>
       <c r="B39">
-        <v>-0.5497577098212645</v>
+        <v>-0.1726927221574073</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>44706</v>
+        <v>41866</v>
       </c>
       <c r="B40">
-        <v>1.775201599534199</v>
+        <v>-0.1729977607768376</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>44798</v>
+        <v>41958</v>
       </c>
       <c r="B41">
-        <v>0.7199425862606432</v>
+        <v>1.050807574684342</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>44890</v>
+        <v>42050</v>
       </c>
       <c r="B42">
-        <v>0.5016525134024334</v>
+        <v>0.5056288600178789</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>44981</v>
+        <v>42139</v>
       </c>
       <c r="B43">
-        <v>-0.5890802842202163</v>
+        <v>-0.2184803162966205</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>45071</v>
+        <v>42231</v>
       </c>
       <c r="B44">
-        <v>-1.005803602395417</v>
+        <v>0.7235341094351355</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>45163</v>
+        <v>42323</v>
       </c>
       <c r="B45">
-        <v>0.5789791938159112</v>
+        <v>0.8513884674671885</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>45254</v>
+        <v>42415</v>
       </c>
       <c r="B46">
-        <v>-0.3682387698544858</v>
+        <v>0.8066734233961483</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>45345</v>
+        <v>42505</v>
       </c>
       <c r="B47">
-        <v>-0.2885446736570572</v>
+        <v>-0.1388227614901609</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>45436</v>
+        <v>42597</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>0.4819278240608753</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>45534</v>
+        <v>42689</v>
       </c>
       <c r="B49">
-        <v>0.009541324901121584</v>
+        <v>0.6629265129002277</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>45618</v>
+        <v>42781</v>
       </c>
       <c r="B50">
-        <v>1.028868575076984</v>
+        <v>0.1646390629436354</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>45713</v>
+        <v>42870</v>
       </c>
       <c r="B51">
-        <v>1.007059757688495</v>
+        <v>1.164700738417963</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>45800</v>
+        <v>42962</v>
       </c>
       <c r="B52">
-        <v>-0.5319104727235242</v>
+        <v>0.4317240674915439</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>45891</v>
+        <v>43054</v>
       </c>
       <c r="B53">
-        <v>0.4200898674779694</v>
+        <v>0.1359170431485039</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="2">
+        <v>43146</v>
+      </c>
+      <c r="B54">
+        <v>0.3857269132374052</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="2">
+        <v>43235</v>
+      </c>
+      <c r="B55">
+        <v>0.876336956515118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="2">
+        <v>43327</v>
+      </c>
+      <c r="B56">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="2">
+        <v>43419</v>
+      </c>
+      <c r="B57">
+        <v>0.008724159582257585</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="2">
+        <v>43511</v>
+      </c>
+      <c r="B58">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="2">
+        <v>43600</v>
+      </c>
+      <c r="B59">
+        <v>0.4878538807911497</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="2">
+        <v>43692</v>
+      </c>
+      <c r="B60">
+        <v>-0.4043302599539206</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="2">
+        <v>43784</v>
+      </c>
+      <c r="B61">
+        <v>0.7183553771707381</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="2">
+        <v>43876</v>
+      </c>
+      <c r="B62">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="2">
+        <v>43966</v>
+      </c>
+      <c r="B63">
+        <v>-7.231044133207007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B64">
+        <v>4.729401638091318</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="2">
+        <v>44150</v>
+      </c>
+      <c r="B65">
+        <v>-0.8905127363963885</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="2">
+        <v>44242</v>
+      </c>
+      <c r="B66">
+        <v>-2.04269378128221</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="2">
+        <v>44331</v>
+      </c>
+      <c r="B67">
+        <v>2.093024636165651</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="2">
+        <v>44423</v>
+      </c>
+      <c r="B68">
+        <v>1.098535546956398</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2">
+        <v>44515</v>
+      </c>
+      <c r="B69">
+        <v>-0.4717175472572421</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2">
+        <v>44607</v>
+      </c>
+      <c r="B70">
+        <v>0.9401304606753627</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2">
+        <v>44696</v>
+      </c>
+      <c r="B71">
+        <v>0.6392725048137464</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="2">
+        <v>44788</v>
+      </c>
+      <c r="B72">
+        <v>0.06357296580725347</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="2">
+        <v>44880</v>
+      </c>
+      <c r="B73">
+        <v>-1.012166871044968</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="2">
+        <v>44972</v>
+      </c>
+      <c r="B74">
+        <v>-0.5703626997413522</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="2">
+        <v>45061</v>
+      </c>
+      <c r="B75">
+        <v>0.2394101325822788</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="2">
+        <v>45153</v>
+      </c>
+      <c r="B76">
+        <v>-0.04072131480353391</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="2">
+        <v>45245</v>
+      </c>
+      <c r="B77">
+        <v>-0.07958838003274593</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="2">
+        <v>45337</v>
+      </c>
+      <c r="B78">
+        <v>0.02912383308249389</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="2">
+        <v>45427</v>
+      </c>
+      <c r="B79">
+        <v>-0.1311265493919933</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="2">
+        <v>45519</v>
+      </c>
+      <c r="B80">
+        <v>-0.03907468377752821</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="2">
+        <v>45611</v>
+      </c>
+      <c r="B81">
+        <v>0.1771324545010202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="2">
+        <v>45703</v>
+      </c>
+      <c r="B82">
+        <v>0.4946531409412387</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2">
+        <v>45792</v>
+      </c>
+      <c r="B83">
+        <v>0.202428137729683</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="2">
+        <v>45884</v>
+      </c>
+      <c r="B84">
+        <v>0.208573386070384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>